<commit_message>
EPBDS-10912 Set ruleservice.instantiation.strategy.lazy=false by default
</commit_message>
<xml_diff>
--- a/ITEST/itest.swaggerSchemas/openl-repository/deployments/rules-service-name-with-spaces/MAIN.xlsx
+++ b/ITEST/itest.swaggerSchemas/openl-repository/deployments/rules-service-name-with-spaces/MAIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.swaggerSchemas\openl-repository\deployments\rules-service-name-with-spaces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\ITEST\itest.swaggerSchemas\openl-repository\deployments\rules-service-name-with-spaces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F4D4DC-8D58-4E3D-8262-D10C1C7756B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCBDD95-42DA-4315-88BC-14BC93566E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="450" windowWidth="28845" windowHeight="20115" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Method String bar(SumTwoDoublesRequest bar)</t>
   </si>
   <si>
-    <t>retirn bar.foo;</t>
-  </si>
-  <si>
     <t>Method Double sumTwoDoubles(Double a, Double b)</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>rules-service-name-with-spaces-datatypes</t>
+  </si>
+  <si>
+    <t>return bar.foo;</t>
   </si>
 </sst>
 </file>
@@ -109,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -125,9 +125,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +165,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -271,7 +271,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:B14"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -458,7 +458,7 @@
   <sheetData>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
@@ -489,7 +489,7 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>